<commit_message>
v. 3.0.4 (Se retoma el proyecto)
</commit_message>
<xml_diff>
--- a/inventarioApp/bdDependencias/2021-04-24 Dependencias IEE.xlsx
+++ b/inventarioApp/bdDependencias/2021-04-24 Dependencias IEE.xlsx
@@ -7,14 +7,14 @@
     <sheet state="visible" name="PRIMARIA" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">SECUNDARIA!$A$1:$E$125</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">SECUNDARIA!$A$1:$E$126</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="191">
   <si>
     <t>DEPENDENCIA</t>
   </si>
@@ -145,6 +145,12 @@
     <t>S1 A201 (Sala de Profesores)</t>
   </si>
   <si>
+    <t>Luis Fernando Ochoa Muñoz</t>
+  </si>
+  <si>
+    <t>S1 A201-A (Cruz Roja)</t>
+  </si>
+  <si>
     <t>S1 A202-A (Rectoria)</t>
   </si>
   <si>
@@ -157,6 +163,9 @@
     <t>S1 A202-B (Secretaría)</t>
   </si>
   <si>
+    <t>María Ofelia Barrera Jaramillo</t>
+  </si>
+  <si>
     <t>S1 A202-C (Almacén Secretaría)</t>
   </si>
   <si>
@@ -178,9 +187,6 @@
     <t>S1 A206 (Coordinacion)</t>
   </si>
   <si>
-    <t>Luis Fernando Ochoa Muñoz</t>
-  </si>
-  <si>
     <t>S1 A207</t>
   </si>
   <si>
@@ -379,7 +385,7 @@
     <t>S1 B206</t>
   </si>
   <si>
-    <t>Cralos Hincapie</t>
+    <t>Carlos Hincapie</t>
   </si>
   <si>
     <t>S1 B207 (Baños hombres y mujeres)</t>
@@ -587,7 +593,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -603,8 +609,12 @@
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -617,6 +627,12 @@
         <bgColor rgb="FF6FA8DC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -624,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -639,6 +655,9 @@
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -890,7 +909,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <f t="shared" ref="A2:A125" si="1">IF(B2="","",A1+1)</f>
+        <f t="shared" ref="A2:A126" si="1">IF(B2="","",A1+1)</f>
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1251,23 +1270,29 @@
       <c r="C25" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="D25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="4">
+        <v>7.1655142E7</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>43</v>
+      <c r="B26" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="E26" s="3">
-        <v>7.1379517E7</v>
+        <v>1.04032627E9</v>
       </c>
     </row>
     <row r="27">
@@ -1276,16 +1301,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="E27" s="3">
-        <v>1.04032627E9</v>
+        <v>7.1379517E7</v>
       </c>
     </row>
     <row r="28">
@@ -1294,16 +1319,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="3">
-        <v>1.04032627E9</v>
+        <v>46</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="6">
+        <v>4.3360172E7</v>
       </c>
     </row>
     <row r="29">
@@ -1312,10 +1337,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>13</v>
@@ -1330,16 +1355,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30" s="4">
-        <v>7.178465E7</v>
+      <c r="E30" s="6">
+        <v>4.3360172E7</v>
       </c>
     </row>
     <row r="31">
@@ -1348,16 +1373,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E31" s="4">
-        <v>3.7926145E7</v>
+        <v>7.178465E7</v>
       </c>
     </row>
     <row r="32">
@@ -1366,16 +1391,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E32" s="4">
-        <v>7.1655142E7</v>
+        <v>3.7926145E7</v>
       </c>
     </row>
     <row r="33">
@@ -1384,16 +1409,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E33" s="4">
-        <v>3.2323443E7</v>
+        <v>7.1655142E7</v>
       </c>
     </row>
     <row r="34">
@@ -1411,7 +1436,7 @@
         <v>58</v>
       </c>
       <c r="E34" s="4">
-        <v>6.3561749E7</v>
+        <v>3.2323443E7</v>
       </c>
     </row>
     <row r="35">
@@ -1429,7 +1454,7 @@
         <v>60</v>
       </c>
       <c r="E35" s="4">
-        <v>1.032070334E9</v>
+        <v>6.3561749E7</v>
       </c>
     </row>
     <row r="36">
@@ -1447,7 +1472,7 @@
         <v>62</v>
       </c>
       <c r="E36" s="4">
-        <v>1.2021698E7</v>
+        <v>1.032070334E9</v>
       </c>
     </row>
     <row r="37">
@@ -1461,6 +1486,12 @@
       <c r="C37" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D37" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="4">
+        <v>1.2021698E7</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="2">
@@ -1468,10 +1499,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39">
@@ -1480,7 +1511,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>5</v>
@@ -1492,16 +1523,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E40" s="4">
-        <v>4.3579902E7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41">
@@ -1516,7 +1541,7 @@
         <v>35</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E41" s="4">
         <v>4.3579902E7</v>
@@ -1528,16 +1553,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="E42" s="4">
-        <v>9.849324E7</v>
+        <v>4.3579902E7</v>
       </c>
     </row>
     <row r="43">
@@ -1545,7 +1570,7 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="3" t="s">
         <v>71</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -1554,8 +1579,8 @@
       <c r="D43" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E43" s="3">
-        <v>4.3344582E7</v>
+      <c r="E43" s="4">
+        <v>9.849324E7</v>
       </c>
     </row>
     <row r="44">
@@ -1573,7 +1598,7 @@
         <v>74</v>
       </c>
       <c r="E44" s="3">
-        <v>7.9606063E7</v>
+        <v>4.3344582E7</v>
       </c>
     </row>
     <row r="45">
@@ -1585,10 +1610,10 @@
         <v>75</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E45" s="3">
         <v>7.9606063E7</v>
@@ -1599,17 +1624,17 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E46" s="4">
-        <v>1.035831101E9</v>
+      <c r="E46" s="3">
+        <v>7.9606063E7</v>
       </c>
     </row>
     <row r="47">
@@ -1623,6 +1648,12 @@
       <c r="C47" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="D47" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" s="4">
+        <v>1.035831101E9</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="2">
@@ -1630,7 +1661,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>35</v>
@@ -1642,7 +1673,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>35</v>
@@ -1654,16 +1685,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E50" s="4">
-        <v>3.255508E7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51">
@@ -1681,7 +1706,7 @@
         <v>84</v>
       </c>
       <c r="E51" s="4">
-        <v>7.3135461E7</v>
+        <v>3.255508E7</v>
       </c>
     </row>
     <row r="52">
@@ -1699,7 +1724,7 @@
         <v>86</v>
       </c>
       <c r="E52" s="4">
-        <v>7.097547E7</v>
+        <v>7.3135461E7</v>
       </c>
     </row>
     <row r="53">
@@ -1717,7 +1742,7 @@
         <v>88</v>
       </c>
       <c r="E53" s="4">
-        <v>9.8636197E7</v>
+        <v>7.097547E7</v>
       </c>
     </row>
     <row r="54">
@@ -1735,7 +1760,7 @@
         <v>90</v>
       </c>
       <c r="E54" s="4">
-        <v>1.013597927E9</v>
+        <v>9.8636197E7</v>
       </c>
     </row>
     <row r="55">
@@ -1747,10 +1772,13 @@
         <v>91</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>72</v>
+        <v>92</v>
+      </c>
+      <c r="E55" s="4">
+        <v>1.013597927E9</v>
       </c>
     </row>
     <row r="56">
@@ -1759,10 +1787,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="57">
@@ -1771,7 +1802,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>5</v>
@@ -1783,16 +1814,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E58" s="4">
-        <v>8005118.0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59">
@@ -1810,7 +1835,7 @@
         <v>97</v>
       </c>
       <c r="E59" s="4">
-        <v>4.3579902E7</v>
+        <v>8005118.0</v>
       </c>
     </row>
     <row r="60">
@@ -1818,17 +1843,17 @@
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E60" s="3">
-        <v>9.8396892E7</v>
+      <c r="E60" s="4">
+        <v>4.3579902E7</v>
       </c>
     </row>
     <row r="61">
@@ -1843,7 +1868,7 @@
         <v>35</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E61" s="3">
         <v>9.8396892E7</v>
@@ -1854,14 +1879,14 @@
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="E62" s="3">
         <v>9.8396892E7</v>
@@ -1873,10 +1898,16 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>35</v>
+        <v>12</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E63" s="3">
+        <v>9.8396892E7</v>
       </c>
     </row>
     <row r="64">
@@ -1885,7 +1916,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>35</v>
@@ -1897,10 +1928,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="66">
@@ -1909,13 +1940,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67">
@@ -1924,10 +1952,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>35</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="68">
@@ -1936,10 +1967,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="69">
@@ -1948,16 +1979,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E69" s="4">
-        <v>9.8572464E7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70">
@@ -1969,7 +1994,13 @@
         <v>110</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>35</v>
+        <v>12</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E70" s="4">
+        <v>9.8572464E7</v>
       </c>
     </row>
     <row r="71">
@@ -1978,7 +2009,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>35</v>
@@ -1990,10 +2021,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="73">
@@ -2002,10 +2033,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74">
@@ -2014,16 +2045,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E74" s="4">
-        <v>4.3142967E7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="75">
@@ -2041,7 +2066,7 @@
         <v>117</v>
       </c>
       <c r="E75" s="4">
-        <v>1.5509745E7</v>
+        <v>4.3142967E7</v>
       </c>
     </row>
     <row r="76">
@@ -2053,10 +2078,14 @@
         <v>118</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E76" s="4">
+        <v>1.5509745E7</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="2">
@@ -2064,7 +2093,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>5</v>
@@ -2078,17 +2107,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E78" s="4">
-        <v>9.8468624E7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
     </row>
     <row r="79">
       <c r="A79" s="2">
@@ -2099,10 +2124,14 @@
         <v>122</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E79" s="4">
+        <v>9.8468624E7</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="2">
@@ -2110,7 +2139,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>5</v>
@@ -2124,7 +2153,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>5</v>
@@ -2137,15 +2166,13 @@
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="B82" s="5" t="s">
-        <v>125</v>
+      <c r="B82" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>126</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D82" s="3"/>
       <c r="E82" s="3"/>
     </row>
     <row r="83">
@@ -2153,13 +2180,15 @@
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="5" t="s">
         <v>127</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D83" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>128</v>
+      </c>
       <c r="E83" s="3"/>
     </row>
     <row r="84">
@@ -2168,7 +2197,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>5</v>
@@ -2182,7 +2211,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>5</v>
@@ -2196,11 +2225,13 @@
         <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>44</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
     </row>
     <row r="87">
       <c r="A87" s="2">
@@ -2208,10 +2239,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="88">
@@ -2220,7 +2251,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>5</v>
@@ -2232,10 +2263,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90">
@@ -2244,16 +2275,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E90" s="3">
-        <v>2.1714453E7</v>
+        <v>46</v>
       </c>
     </row>
     <row r="91">
@@ -2265,7 +2290,13 @@
         <v>136</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E91" s="3">
+        <v>2.1714453E7</v>
       </c>
     </row>
     <row r="92">
@@ -2274,16 +2305,10 @@
         <v>91</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E92" s="4">
-        <v>2.171391E7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93">
@@ -2301,7 +2326,7 @@
         <v>140</v>
       </c>
       <c r="E93" s="4">
-        <v>2.1714513E7</v>
+        <v>2.171391E7</v>
       </c>
     </row>
     <row r="94">
@@ -2319,7 +2344,7 @@
         <v>142</v>
       </c>
       <c r="E94" s="4">
-        <v>4.3634714E7</v>
+        <v>2.1714513E7</v>
       </c>
     </row>
     <row r="95">
@@ -2331,7 +2356,13 @@
         <v>143</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E95" s="4">
+        <v>4.3634714E7</v>
       </c>
     </row>
     <row r="96">
@@ -2340,7 +2371,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>5</v>
@@ -2352,7 +2383,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>5</v>
@@ -2364,7 +2395,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>5</v>
@@ -2376,7 +2407,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>5</v>
@@ -2388,7 +2419,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>5</v>
@@ -2400,16 +2431,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E101" s="4">
-        <v>1.035831101E9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102">
@@ -2418,16 +2443,16 @@
         <v>101</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="E102" s="4">
-        <v>3.227645E7</v>
+        <v>1.035831101E9</v>
       </c>
     </row>
     <row r="103">
@@ -2439,7 +2464,13 @@
         <v>152</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>35</v>
+        <v>12</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E103" s="4">
+        <v>3.227645E7</v>
       </c>
     </row>
     <row r="104">
@@ -2448,7 +2479,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>35</v>
@@ -2460,7 +2491,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>35</v>
@@ -2472,16 +2503,10 @@
         <v>105</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E106" s="3">
-        <v>1.044502519E9</v>
       </c>
     </row>
     <row r="107">
@@ -2496,7 +2521,7 @@
         <v>35</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E107" s="3">
         <v>1.044502519E9</v>
@@ -2508,16 +2533,16 @@
         <v>107</v>
       </c>
       <c r="B108" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D108" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C108" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E108" s="4">
-        <v>2.1715063E7</v>
+      <c r="E108" s="3">
+        <v>1.044502519E9</v>
       </c>
     </row>
     <row r="109">
@@ -2529,13 +2554,13 @@
         <v>160</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E109" s="3">
-        <v>1.044502519E9</v>
+        <v>161</v>
+      </c>
+      <c r="E109" s="4">
+        <v>2.1715063E7</v>
       </c>
     </row>
     <row r="110">
@@ -2544,16 +2569,16 @@
         <v>109</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E110" s="4">
-        <v>4.3365654E7</v>
+        <v>158</v>
+      </c>
+      <c r="E110" s="3">
+        <v>1.044502519E9</v>
       </c>
     </row>
     <row r="111">
@@ -2565,13 +2590,13 @@
         <v>163</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>164</v>
       </c>
       <c r="E111" s="4">
-        <v>3.2228815E7</v>
+        <v>4.3365654E7</v>
       </c>
     </row>
     <row r="112">
@@ -2589,7 +2614,7 @@
         <v>166</v>
       </c>
       <c r="E112" s="4">
-        <v>4.336296E7</v>
+        <v>3.2228815E7</v>
       </c>
     </row>
     <row r="113">
@@ -2607,7 +2632,7 @@
         <v>168</v>
       </c>
       <c r="E113" s="4">
-        <v>1.5483504E7</v>
+        <v>4.336296E7</v>
       </c>
     </row>
     <row r="114">
@@ -2619,7 +2644,13 @@
         <v>169</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E114" s="4">
+        <v>1.5483504E7</v>
       </c>
     </row>
     <row r="115">
@@ -2628,7 +2659,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>5</v>
@@ -2640,7 +2671,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>5</v>
@@ -2652,16 +2683,10 @@
         <v>116</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E117" s="4">
-        <v>2.4398628E7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118">
@@ -2676,10 +2701,10 @@
         <v>12</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E118" s="3">
-        <v>1.044502519E9</v>
+        <v>175</v>
+      </c>
+      <c r="E118" s="4">
+        <v>2.4398628E7</v>
       </c>
     </row>
     <row r="119">
@@ -2688,16 +2713,16 @@
         <v>118</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="E119" s="4">
-        <v>4.3760828E7</v>
+        <v>158</v>
+      </c>
+      <c r="E119" s="3">
+        <v>1.044502519E9</v>
       </c>
     </row>
     <row r="120">
@@ -2709,7 +2734,13 @@
         <v>177</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>35</v>
+        <v>12</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E120" s="4">
+        <v>4.3760828E7</v>
       </c>
     </row>
     <row r="121">
@@ -2718,10 +2749,10 @@
         <v>120</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="122">
@@ -2730,16 +2761,10 @@
         <v>121</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D122" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="E122" s="4">
-        <v>3.2277506E7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="123">
@@ -2751,7 +2776,13 @@
         <v>181</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E123" s="4">
+        <v>3.2277506E7</v>
       </c>
     </row>
     <row r="124">
@@ -2760,10 +2791,10 @@
         <v>123</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125">
@@ -2772,21 +2803,33 @@
         <v>124</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C125" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="2">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C126" s="3" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$E$125">
-    <sortState ref="A1:E125">
-      <sortCondition ref="B1:B125"/>
-      <sortCondition ref="D1:D125"/>
+  <autoFilter ref="$A$1:$E$126">
+    <sortState ref="A1:E126">
+      <sortCondition ref="B1:B126"/>
+      <sortCondition ref="D1:D126"/>
     </sortState>
   </autoFilter>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C125">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C126">
       <formula1>"Salón,Oficina,Departamento,Otro Lugar"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2833,10 +2876,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3">
@@ -2845,7 +2888,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
@@ -2857,7 +2900,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
@@ -2869,10 +2912,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6">
@@ -2881,13 +2924,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7">
@@ -2896,7 +2939,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
@@ -2908,13 +2951,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9">
@@ -2923,13 +2966,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10">
@@ -2938,13 +2981,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11">
@@ -2953,7 +2996,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>5</v>
@@ -2965,7 +3008,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>5</v>
@@ -2977,7 +3020,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>5</v>
@@ -2989,7 +3032,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>5</v>
@@ -3001,7 +3044,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>5</v>
@@ -3013,7 +3056,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>5</v>
@@ -3025,13 +3068,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18">
@@ -3040,13 +3083,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19">
@@ -3055,7 +3098,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>35</v>
@@ -3067,7 +3110,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>35</v>
@@ -3079,7 +3122,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>35</v>
@@ -3091,13 +3134,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23">
@@ -3106,7 +3149,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>35</v>
@@ -3118,13 +3161,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25">
@@ -3133,13 +3176,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26">
@@ -3148,13 +3191,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27">
@@ -3163,13 +3206,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28">
@@ -3178,7 +3221,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>5</v>
@@ -3190,7 +3233,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>5</v>
@@ -3202,13 +3245,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31">
@@ -3217,13 +3260,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32">
@@ -3232,13 +3275,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33">
@@ -3247,7 +3290,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>35</v>
@@ -3259,7 +3302,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>5</v>
@@ -3271,13 +3314,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36">
@@ -3286,7 +3329,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>5</v>
@@ -3298,7 +3341,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>35</v>
@@ -3310,7 +3353,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>5</v>

</xml_diff>